<commit_message>
Fixed some graph titles
</commit_message>
<xml_diff>
--- a/data/tree-mureco.xlsx
+++ b/data/tree-mureco.xlsx
@@ -624,14 +624,14 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Utility</a:t>
+              <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Maximal Utility over Iteration for Parameters of Function Trees</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> over Iteration for Trees</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-US">
+              <a:effectLst/>
+            </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
@@ -2096,11 +2096,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="45863680"/>
-        <c:axId val="45983232"/>
+        <c:axId val="78658944"/>
+        <c:axId val="78661120"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="45863680"/>
+        <c:axId val="78658944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2128,7 +2128,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45983232"/>
+        <c:crossAx val="78661120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2136,7 +2136,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="45983232"/>
+        <c:axId val="78661120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1000"/>
@@ -2156,7 +2156,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Utility</a:t>
+                  <a:t>Maximal Utility</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -2168,7 +2168,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45863680"/>
+        <c:crossAx val="78658944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2515,7 +2515,7 @@
   <dimension ref="A1:O26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="Q20" sqref="Q20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>